<commit_message>
More words words words
</commit_message>
<xml_diff>
--- a/waffle_results.xlsx
+++ b/waffle_results.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,17 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david.lively/dev/github/GoLightly/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{081D74DC-F25F-AF41-BE65-2F9AEAF24751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA33841B-C85F-2349-BF85-CAC4E2CDE779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" activeTab="1"/>
+    <workbookView xWindow="9260" yWindow="2440" windowWidth="35840" windowHeight="21900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="export" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -44,7 +41,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1713,9 +1710,9 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>800100</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1742,265 +1739,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="trash"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="1">
-          <cell r="E1" t="str">
-            <v>maxValue</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="B2">
-            <v>480</v>
-          </cell>
-          <cell r="E2">
-            <v>8.6314659999999996</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="B3">
-            <v>544</v>
-          </cell>
-          <cell r="E3">
-            <v>17.319019999999998</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="B4">
-            <v>608</v>
-          </cell>
-          <cell r="E4">
-            <v>13.95567</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="B5">
-            <v>672</v>
-          </cell>
-          <cell r="E5">
-            <v>13.33652</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="B6">
-            <v>736</v>
-          </cell>
-          <cell r="E6">
-            <v>7.5201130000000003</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="B7">
-            <v>800</v>
-          </cell>
-          <cell r="E7">
-            <v>8.5000979999999995</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="B8">
-            <v>864</v>
-          </cell>
-          <cell r="E8">
-            <v>9.9405380000000001</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="B9">
-            <v>928</v>
-          </cell>
-          <cell r="E9">
-            <v>8.7069489999999998</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="B10">
-            <v>992</v>
-          </cell>
-          <cell r="E10">
-            <v>5.5007060000000001</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="B11">
-            <v>1056</v>
-          </cell>
-          <cell r="E11">
-            <v>9.0897210000000008</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="B12">
-            <v>1120</v>
-          </cell>
-          <cell r="E12">
-            <v>9.9005410000000005</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="B13">
-            <v>1184</v>
-          </cell>
-          <cell r="E13">
-            <v>8.0280640000000005</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="B14">
-            <v>1248</v>
-          </cell>
-          <cell r="E14">
-            <v>8.2926610000000007</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="B15">
-            <v>1312</v>
-          </cell>
-          <cell r="E15">
-            <v>8.2506979999999999</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="B16">
-            <v>1376</v>
-          </cell>
-          <cell r="E16">
-            <v>8.4396509999999996</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="B17">
-            <v>1440</v>
-          </cell>
-          <cell r="E17">
-            <v>6.7653509999999999</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="B18">
-            <v>1504</v>
-          </cell>
-          <cell r="E18">
-            <v>5.9363409999999996</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="B19">
-            <v>1568</v>
-          </cell>
-          <cell r="E19">
-            <v>6.1986090000000003</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="B20">
-            <v>1632</v>
-          </cell>
-          <cell r="E20">
-            <v>5.8807679999999998</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="B21">
-            <v>1696.001</v>
-          </cell>
-          <cell r="E21">
-            <v>5.5119300000000004</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="B22">
-            <v>1760.001</v>
-          </cell>
-          <cell r="E22">
-            <v>5.5289029999999997</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="B23">
-            <v>1824.001</v>
-          </cell>
-          <cell r="E23">
-            <v>5.8760510000000004</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="B24">
-            <v>1888.001</v>
-          </cell>
-          <cell r="E24">
-            <v>4.7621380000000002</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="B25">
-            <v>1952.001</v>
-          </cell>
-          <cell r="E25">
-            <v>5.1622450000000004</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="B26">
-            <v>2016.001</v>
-          </cell>
-          <cell r="E26">
-            <v>6.0030200000000002</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="B27">
-            <v>2080</v>
-          </cell>
-          <cell r="E27">
-            <v>5.0304679999999999</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="B28">
-            <v>2144</v>
-          </cell>
-          <cell r="E28">
-            <v>4.8073870000000003</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="B29">
-            <v>2208</v>
-          </cell>
-          <cell r="E29">
-            <v>4.5140269999999996</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="B30">
-            <v>2272</v>
-          </cell>
-          <cell r="E30">
-            <v>4.2398550000000004</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="B31">
-            <v>2336</v>
-          </cell>
-          <cell r="E31">
-            <v>3.9702899999999999</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2299,7 +2037,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
@@ -2841,7 +2579,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">

</xml_diff>